<commit_message>
PROS-5313 Survey update JNJIT
</commit_message>
<xml_diff>
--- a/Projects/JNJIT/Data/SurveyTemplate.xlsx
+++ b/Projects/JNJIT/Data/SurveyTemplate.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t xml:space="preserve">Question_Text</t>
   </si>
@@ -34,97 +34,52 @@
     <t xml:space="preserve">branded, visible &amp; accessible</t>
   </si>
   <si>
-    <t xml:space="preserve">Quanti Espositori / Fuori scaffale Baby JnJ sono presenti all'interno del punto vendita? (incluso Manhattan, gondole, testate, cestoni)</t>
+    <t xml:space="preserve">Quanti Manhattan, gondole, testate e/o cestoni Baby JnJ sono presenti all'interno del punto vendita?</t>
   </si>
   <si>
     <t xml:space="preserve">Total Secondary Placements</t>
   </si>
   <si>
-    <t xml:space="preserve">Quanti Espositori / Fuori scaffali Baby JnJ sono presenti all'entrata del punto vendita?</t>
+    <t xml:space="preserve">Quanti Espositori / Fuori scaffale Beauty JnJ brandizzati e accessibili sono presenti all'interno del punto vendita?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quanti Manhattan, gondole, testate e/o cestoni Beauty JnJ sono presenti all'interno del punto vendita?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quanti Espositori / Fuori scaffale Fem Care JnJ brandizzati e accessibili sono presenti all'interno del punto vendita?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quanti Manhattan, gondole, testate e/o cestoni Fem Care JnJ sono presenti all'interno del punto vendita?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quanti Espositori / Fuori scaffale Listerine brandizzati e accessibili sono presenti all'interno del punto vendita?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quanti Manhattan, gondole, testate e/o cestoni Listerine sono presenti all'interno del punto vendita?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quanti Espositori / Fuori scaffale OTC brandizzati e accessibili sono presenti all'interno del punto vendita?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quanti Manhattan, gondole, testate e/o cestoni OTC JnJ sono presenti all'interno del punto vendita?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quanti Espositori / Fuori scaffali Baby JnJ sono presenti nelle aree GOLD? (Area GOLD si intende: entrata, corridoio principale, zone in prossimità delle casse)</t>
   </si>
   <si>
     <t xml:space="preserve">Gold location</t>
   </si>
   <si>
-    <t xml:space="preserve">Quanti Espositori / Fuori scaffali Baby JnJ sono presenti vicino la cassa?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quanti Espositori / Fuori scaffali Baby JnJ sono presenti lungo il corridoio principale?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quanti Espositori / Fuori scaffali Baby JnJ sono presenti nell'area GOLD?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quanti Espositori / Fuori scaffale Beauty JnJ brandizzati e accessibili sono presenti all'interno del punto vendita?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quanti Espositori / Fuori scaffale Beauty JnJ sono presenti all'interno del punto vendita? ((incluso Manhattan, gondole, testate, cestoni))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quanti Espositori / Fuori scaffali Beauty JnJ sono presenti all'entrata del punto vendita?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quanti Espositori / Fuori scaffali Beauty JnJsono presenti vicino la cassa?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quanti espositori Beauty JnJ sono presenti lungo il corridoio principale?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quanti Espositori / Fuori scaffali Beauty JnJ sono presenti nell'area GOLD?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quanti Espositori / Fuori scaffale Fem Care JnJ brandizzati e accessibili sono presenti all'interno del punto vendita?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quanti Espositori / Fuori scaffale Fem Care JnJ sono presenti all'interno del punto vendita? ((incluso Manhattan, gondole, testate, cestoni))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quanti Espositori / Fuori scaffali Fem Care JnJ sono presenti all'entrata del punto vendita?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quanti Espositori / Fuori scaffali Fem Care JnJsono presenti vicino la cassa?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quanti Espositori / Fuori scaffali Fem Care JnJ sono presenti lungo il corridoio principale?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quanti Espositori / Fuori scaffali Fem Care JnJ sono presenti nell'area GOLD?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quanti Espositori / Fuori scaffale Listerine brandizzati e accessibili sono presenti all'interno del punto vendita?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quanti Espositori / Fuori scaffale Listerine sono presenti all'interno del punto vendita? (incluso Manhattan, gondole, testate, cestoni))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quanti Espositori / fuori scaffali Listerine sono presenti all'entrata del punto vendita?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quanti Espositori / fuori scaffali Listerine sono presenti vicino la cassa?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quanti Espositori / Fuori scaffali listerine sono presenti lungo il corridoio principale?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quanti Espositori / Fuori scaffali Listerine sono presenti nell'area GOLD?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quanti Espositori / Fuori scaffale OTC brandizzati e accessibili sono presenti all'interno del punto vendita?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quanti Espositori / Fuori scaffale OTC sono presenti all'interno del punto vendita? (incluso Manhattan, gondole, testate, cestoni))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quanti Espositori / Fuori scaffali OTC JnJ sono presenti all'entrata del punto vendita?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quanti Espositori / Fuori scaffali OTC JnJ sono presenti vicino la cassa/ sul bancone del punto vendita?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quanti Espositori / Fuori scaffali OTC JnJ sono presenti lungo il corridoio principale?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quanti espositori OTC JnJ sono presenti nell'area GOLD?</t>
+    <t xml:space="preserve">Quanti Espositori / Fuori scaffali BEAUTY JnJ sono presenti nelle aree GOLD? (Area GOLD si intende: entrata, corridoio principale, zone in prossimità delle casse)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quanti Espositori / Fuori scaffali Fem CARE JnJ sono presenti nelle aree GOLD? (Area GOLD si intende: entrata, corridoio principale, zone in prossimità delle casse)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quanti Espositori / Fuori scaffali Listerine JnJ sono presenti nelle aree GOLD? (Area GOLD si intende: entrata, corridoio principale, zone in prossimità delle casse)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quanti Espositori / Fuori scaffali OTC JnJ sono presenti nelle aree GOLD? (Area GOLD si intende: entrata, corridoio principale, zone in prossimità delle casse)</t>
   </si>
 </sst>
 </file>
@@ -239,14 +194,15 @@
   <dimension ref="A1:C65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H28" activeCellId="0" sqref="H28"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="104.602040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.2040816326531"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.5"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="137.918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.6581632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.48469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -280,40 +236,40 @@
         <v>6</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>3</v>
@@ -321,7 +277,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>5</v>
@@ -329,26 +285,26 @@
     </row>
     <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -356,7 +312,7 @@
         <v>16</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -364,7 +320,7 @@
         <v>17</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -372,7 +328,7 @@
         <v>18</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -380,127 +336,7 @@
         <v>19</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B30" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B31" s="0" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="1048569" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>